<commit_message>
Change times for ESP32
</commit_message>
<xml_diff>
--- a/Measures/NC46_400/pwm2speed.xlsx
+++ b/Measures/NC46_400/pwm2speed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\source\repos\RotatingTable.Arduino\Measures\NC46_400\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1A99827-C3A2-45AF-9440-BB3751A172C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D508B9-4EB4-424A-9CE5-9C5FAAA357AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6450" yWindow="255" windowWidth="19770" windowHeight="14895" xr2:uid="{A8659596-E7CE-445D-A5F7-DEEAE94F9AC8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A8659596-E7CE-445D-A5F7-DEEAE94F9AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Times" sheetId="3" r:id="rId1"/>
@@ -196,273 +196,285 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Times!$B$2:$B$89</c:f>
+              <c:f>Times!$B$2:$B$93</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
-                <c:ptCount val="88"/>
+                <c:ptCount val="92"/>
                 <c:pt idx="0">
-                  <c:v>108.27</c:v>
+                  <c:v>99.65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>83.75</c:v>
+                  <c:v>86.91</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70.34</c:v>
+                  <c:v>74.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.57</c:v>
+                  <c:v>62.37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53.6</c:v>
+                  <c:v>56.09</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47.84</c:v>
+                  <c:v>48.96</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43.82</c:v>
+                  <c:v>45.33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>39.96</c:v>
+                  <c:v>40.92</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37.33</c:v>
+                  <c:v>38.24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34.33</c:v>
+                  <c:v>34.79</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>32.299999999999997</c:v>
+                  <c:v>33.06</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>30.24</c:v>
+                  <c:v>30.64</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.69</c:v>
+                  <c:v>29.19</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.92</c:v>
+                  <c:v>27.29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>25.82</c:v>
+                  <c:v>26.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.37</c:v>
+                  <c:v>24.51</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.5</c:v>
+                  <c:v>23.79</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>22.2</c:v>
+                  <c:v>22.45</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>21.6</c:v>
+                  <c:v>21.72</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.49</c:v>
+                  <c:v>20.72</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19.920000000000002</c:v>
+                  <c:v>20.079999999999998</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>18.97</c:v>
+                  <c:v>19.18</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18.579999999999998</c:v>
+                  <c:v>18.68</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>17.72</c:v>
+                  <c:v>17.829999999999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>17.36</c:v>
+                  <c:v>17.48</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>16.61</c:v>
+                  <c:v>16.71</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>16.29</c:v>
+                  <c:v>16.47</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15.66</c:v>
+                  <c:v>15.81</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15.38</c:v>
+                  <c:v>15.52</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>14.81</c:v>
+                  <c:v>14.89</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>14.55</c:v>
+                  <c:v>14.61</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>14.05</c:v>
+                  <c:v>14.16</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>13.83</c:v>
+                  <c:v>13.91</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>13.38</c:v>
+                  <c:v>13.42</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>13.17</c:v>
+                  <c:v>13.23</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>12.8</c:v>
+                  <c:v>12.85</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>12.56</c:v>
+                  <c:v>12.65</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>12.22</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>12.08</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.73</c:v>
+                  <c:v>11.79</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>11.55</c:v>
+                  <c:v>11.62</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>11.28</c:v>
+                  <c:v>11.32</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>11.14</c:v>
+                  <c:v>11.12</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>10.83</c:v>
+                  <c:v>10.87</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>10.67</c:v>
+                  <c:v>10.73</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>10.44</c:v>
+                  <c:v>10.51</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>10.29</c:v>
+                  <c:v>10.41</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>10.07</c:v>
+                  <c:v>10.16</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>9.99</c:v>
+                  <c:v>10.050000000000001</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9.75</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>9.67</c:v>
+                  <c:v>9.66</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>9.44</c:v>
+                  <c:v>9.5399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>9.35</c:v>
+                  <c:v>9.4499999999999993</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>9.19</c:v>
+                  <c:v>9.2799999999999994</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>9.06</c:v>
+                  <c:v>9.17</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>8.93</c:v>
+                  <c:v>9.0399999999999991</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>8.84</c:v>
+                  <c:v>8.99</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>8.6999999999999993</c:v>
+                  <c:v>8.7100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>8.64</c:v>
+                  <c:v>8.67</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>8.4600000000000009</c:v>
+                  <c:v>8.5299999999999994</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>8.36</c:v>
+                  <c:v>8.49</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>8.23</c:v>
+                  <c:v>8.33</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>8.14</c:v>
+                  <c:v>8.3800000000000008</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>8</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>7.95</c:v>
+                  <c:v>8.16</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7.82</c:v>
+                  <c:v>7.85</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>7.79</c:v>
+                  <c:v>7.97</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>7.62</c:v>
+                  <c:v>7.69</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>7.6</c:v>
+                  <c:v>7.76</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>7.38</c:v>
+                  <c:v>7.57</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7.42</c:v>
+                  <c:v>7.59</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>7.24</c:v>
+                  <c:v>7.4</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>7.27</c:v>
+                  <c:v>7.45</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>7.08</c:v>
+                  <c:v>7.14</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>7.09</c:v>
+                  <c:v>7.31</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>6.94</c:v>
+                  <c:v>7.06</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>6.9</c:v>
+                  <c:v>7.12</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>6.8</c:v>
+                  <c:v>6.88</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>6.79</c:v>
+                  <c:v>6.92</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>6.66</c:v>
+                  <c:v>6.71</c:v>
                 </c:pt>
                 <c:pt idx="80">
+                  <c:v>6.84</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>6.55</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>6.61</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>6.48</c:v>
+                </c:pt>
+                <c:pt idx="84">
                   <c:v>6.59</c:v>
                 </c:pt>
-                <c:pt idx="81">
-                  <c:v>6.53</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>6.47</c:v>
-                </c:pt>
-                <c:pt idx="83">
+                <c:pt idx="85">
                   <c:v>6.33</c:v>
                 </c:pt>
-                <c:pt idx="84">
-                  <c:v>6.42</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>6.3</c:v>
-                </c:pt>
                 <c:pt idx="86">
+                  <c:v>6.37</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6.15</c:v>
+                </c:pt>
+                <c:pt idx="88" formatCode="0.00">
                   <c:v>6.21</c:v>
                 </c:pt>
-                <c:pt idx="87">
-                  <c:v>6.17</c:v>
+                <c:pt idx="89" formatCode="0.00">
+                  <c:v>5.96</c:v>
+                </c:pt>
+                <c:pt idx="90" formatCode="0.00">
+                  <c:v>6.12</c:v>
+                </c:pt>
+                <c:pt idx="91" formatCode="0.00">
+                  <c:v>5.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1668,7 +1680,7 @@
   <dimension ref="A1:B197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1689,7 +1701,7 @@
         <v>97</v>
       </c>
       <c r="B2" s="3">
-        <v>108.27</v>
+        <v>99.65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1697,7 +1709,7 @@
         <v>98</v>
       </c>
       <c r="B3" s="3">
-        <v>83.75</v>
+        <v>86.91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1705,7 +1717,7 @@
         <v>99</v>
       </c>
       <c r="B4" s="3">
-        <v>70.34</v>
+        <v>74.61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1713,7 +1725,7 @@
         <v>100</v>
       </c>
       <c r="B5" s="3">
-        <v>60.57</v>
+        <v>62.37</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1721,7 +1733,7 @@
         <v>101</v>
       </c>
       <c r="B6" s="3">
-        <v>53.6</v>
+        <v>56.09</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1729,7 +1741,7 @@
         <v>102</v>
       </c>
       <c r="B7" s="3">
-        <v>47.84</v>
+        <v>48.96</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1737,7 +1749,7 @@
         <v>103</v>
       </c>
       <c r="B8" s="3">
-        <v>43.82</v>
+        <v>45.33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1745,7 +1757,7 @@
         <v>104</v>
       </c>
       <c r="B9" s="3">
-        <v>39.96</v>
+        <v>40.92</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1753,7 +1765,7 @@
         <v>105</v>
       </c>
       <c r="B10" s="3">
-        <v>37.33</v>
+        <v>38.24</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1761,7 +1773,7 @@
         <v>106</v>
       </c>
       <c r="B11" s="3">
-        <v>34.33</v>
+        <v>34.79</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1769,7 +1781,7 @@
         <v>107</v>
       </c>
       <c r="B12" s="3">
-        <v>32.299999999999997</v>
+        <v>33.06</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1777,7 +1789,7 @@
         <v>108</v>
       </c>
       <c r="B13" s="3">
-        <v>30.24</v>
+        <v>30.64</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1785,7 +1797,7 @@
         <v>109</v>
       </c>
       <c r="B14" s="3">
-        <v>28.69</v>
+        <v>29.19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1793,7 +1805,7 @@
         <v>110</v>
       </c>
       <c r="B15" s="3">
-        <v>26.92</v>
+        <v>27.29</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1801,7 +1813,7 @@
         <v>111</v>
       </c>
       <c r="B16" s="3">
-        <v>25.82</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1809,7 +1821,7 @@
         <v>112</v>
       </c>
       <c r="B17" s="3">
-        <v>24.37</v>
+        <v>24.51</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1817,7 +1829,7 @@
         <v>113</v>
       </c>
       <c r="B18" s="3">
-        <v>23.5</v>
+        <v>23.79</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1825,7 +1837,7 @@
         <v>114</v>
       </c>
       <c r="B19" s="3">
-        <v>22.2</v>
+        <v>22.45</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1833,7 +1845,7 @@
         <v>115</v>
       </c>
       <c r="B20" s="3">
-        <v>21.6</v>
+        <v>21.72</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1841,7 +1853,7 @@
         <v>116</v>
       </c>
       <c r="B21" s="3">
-        <v>20.49</v>
+        <v>20.72</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1849,7 +1861,7 @@
         <v>117</v>
       </c>
       <c r="B22" s="3">
-        <v>19.920000000000002</v>
+        <v>20.079999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1857,7 +1869,7 @@
         <v>118</v>
       </c>
       <c r="B23" s="3">
-        <v>18.97</v>
+        <v>19.18</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1865,7 +1877,7 @@
         <v>119</v>
       </c>
       <c r="B24" s="3">
-        <v>18.579999999999998</v>
+        <v>18.68</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1873,7 +1885,7 @@
         <v>120</v>
       </c>
       <c r="B25" s="3">
-        <v>17.72</v>
+        <v>17.829999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1881,7 +1893,7 @@
         <v>121</v>
       </c>
       <c r="B26" s="3">
-        <v>17.36</v>
+        <v>17.48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1889,7 +1901,7 @@
         <v>122</v>
       </c>
       <c r="B27" s="3">
-        <v>16.61</v>
+        <v>16.71</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1897,7 +1909,7 @@
         <v>123</v>
       </c>
       <c r="B28" s="3">
-        <v>16.29</v>
+        <v>16.47</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1905,7 +1917,7 @@
         <v>124</v>
       </c>
       <c r="B29" s="3">
-        <v>15.66</v>
+        <v>15.81</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1913,7 +1925,7 @@
         <v>125</v>
       </c>
       <c r="B30" s="3">
-        <v>15.38</v>
+        <v>15.52</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1921,7 +1933,7 @@
         <v>126</v>
       </c>
       <c r="B31" s="3">
-        <v>14.81</v>
+        <v>14.89</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1929,7 +1941,7 @@
         <v>127</v>
       </c>
       <c r="B32" s="3">
-        <v>14.55</v>
+        <v>14.61</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1937,7 +1949,7 @@
         <v>128</v>
       </c>
       <c r="B33" s="3">
-        <v>14.05</v>
+        <v>14.16</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1945,7 +1957,7 @@
         <v>129</v>
       </c>
       <c r="B34" s="3">
-        <v>13.83</v>
+        <v>13.91</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1953,7 +1965,7 @@
         <v>130</v>
       </c>
       <c r="B35" s="3">
-        <v>13.38</v>
+        <v>13.42</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1961,7 +1973,7 @@
         <v>131</v>
       </c>
       <c r="B36" s="3">
-        <v>13.17</v>
+        <v>13.23</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1969,7 +1981,7 @@
         <v>132</v>
       </c>
       <c r="B37" s="3">
-        <v>12.8</v>
+        <v>12.85</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1977,7 +1989,7 @@
         <v>133</v>
       </c>
       <c r="B38" s="3">
-        <v>12.56</v>
+        <v>12.65</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1985,7 +1997,7 @@
         <v>134</v>
       </c>
       <c r="B39" s="3">
-        <v>12.22</v>
+        <v>12.3</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2001,7 +2013,7 @@
         <v>136</v>
       </c>
       <c r="B41" s="3">
-        <v>11.73</v>
+        <v>11.79</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2009,7 +2021,7 @@
         <v>137</v>
       </c>
       <c r="B42" s="3">
-        <v>11.55</v>
+        <v>11.62</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2017,7 +2029,7 @@
         <v>138</v>
       </c>
       <c r="B43" s="3">
-        <v>11.28</v>
+        <v>11.32</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2025,7 +2037,7 @@
         <v>139</v>
       </c>
       <c r="B44" s="3">
-        <v>11.14</v>
+        <v>11.12</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2033,7 +2045,7 @@
         <v>140</v>
       </c>
       <c r="B45" s="3">
-        <v>10.83</v>
+        <v>10.87</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2041,7 +2053,7 @@
         <v>141</v>
       </c>
       <c r="B46" s="3">
-        <v>10.67</v>
+        <v>10.73</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2049,7 +2061,7 @@
         <v>142</v>
       </c>
       <c r="B47" s="3">
-        <v>10.44</v>
+        <v>10.51</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2057,7 +2069,7 @@
         <v>143</v>
       </c>
       <c r="B48" s="3">
-        <v>10.29</v>
+        <v>10.41</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2065,7 +2077,7 @@
         <v>144</v>
       </c>
       <c r="B49" s="3">
-        <v>10.07</v>
+        <v>10.16</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2073,7 +2085,7 @@
         <v>145</v>
       </c>
       <c r="B50" s="3">
-        <v>9.99</v>
+        <v>10.050000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2081,7 +2093,7 @@
         <v>146</v>
       </c>
       <c r="B51" s="3">
-        <v>9.75</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2089,7 +2101,7 @@
         <v>147</v>
       </c>
       <c r="B52" s="3">
-        <v>9.67</v>
+        <v>9.66</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2097,7 +2109,7 @@
         <v>148</v>
       </c>
       <c r="B53" s="3">
-        <v>9.44</v>
+        <v>9.5399999999999991</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2105,7 +2117,7 @@
         <v>149</v>
       </c>
       <c r="B54" s="3">
-        <v>9.35</v>
+        <v>9.4499999999999993</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2113,7 +2125,7 @@
         <v>150</v>
       </c>
       <c r="B55" s="3">
-        <v>9.19</v>
+        <v>9.2799999999999994</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2121,7 +2133,7 @@
         <v>151</v>
       </c>
       <c r="B56" s="3">
-        <v>9.06</v>
+        <v>9.17</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2129,7 +2141,7 @@
         <v>152</v>
       </c>
       <c r="B57" s="3">
-        <v>8.93</v>
+        <v>9.0399999999999991</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2137,7 +2149,7 @@
         <v>153</v>
       </c>
       <c r="B58" s="3">
-        <v>8.84</v>
+        <v>8.99</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2145,7 +2157,7 @@
         <v>154</v>
       </c>
       <c r="B59" s="3">
-        <v>8.6999999999999993</v>
+        <v>8.7100000000000009</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2153,7 +2165,7 @@
         <v>155</v>
       </c>
       <c r="B60" s="3">
-        <v>8.64</v>
+        <v>8.67</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2161,7 +2173,7 @@
         <v>156</v>
       </c>
       <c r="B61" s="3">
-        <v>8.4600000000000009</v>
+        <v>8.5299999999999994</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2169,7 +2181,7 @@
         <v>157</v>
       </c>
       <c r="B62" s="3">
-        <v>8.36</v>
+        <v>8.49</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2177,7 +2189,7 @@
         <v>158</v>
       </c>
       <c r="B63" s="3">
-        <v>8.23</v>
+        <v>8.33</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2185,7 +2197,7 @@
         <v>159</v>
       </c>
       <c r="B64" s="3">
-        <v>8.14</v>
+        <v>8.3800000000000008</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2193,7 +2205,7 @@
         <v>160</v>
       </c>
       <c r="B65" s="3">
-        <v>8</v>
+        <v>8.1</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2201,7 +2213,7 @@
         <v>161</v>
       </c>
       <c r="B66" s="3">
-        <v>7.95</v>
+        <v>8.16</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2209,7 +2221,7 @@
         <v>162</v>
       </c>
       <c r="B67" s="3">
-        <v>7.82</v>
+        <v>7.85</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2217,7 +2229,7 @@
         <v>163</v>
       </c>
       <c r="B68" s="3">
-        <v>7.79</v>
+        <v>7.97</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2225,7 +2237,7 @@
         <v>164</v>
       </c>
       <c r="B69" s="3">
-        <v>7.62</v>
+        <v>7.69</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2233,7 +2245,7 @@
         <v>165</v>
       </c>
       <c r="B70" s="3">
-        <v>7.6</v>
+        <v>7.76</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2241,7 +2253,7 @@
         <v>166</v>
       </c>
       <c r="B71" s="3">
-        <v>7.38</v>
+        <v>7.57</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2249,7 +2261,7 @@
         <v>167</v>
       </c>
       <c r="B72" s="3">
-        <v>7.42</v>
+        <v>7.59</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2257,7 +2269,7 @@
         <v>168</v>
       </c>
       <c r="B73" s="3">
-        <v>7.24</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2265,7 +2277,7 @@
         <v>169</v>
       </c>
       <c r="B74" s="3">
-        <v>7.27</v>
+        <v>7.45</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2273,7 +2285,7 @@
         <v>170</v>
       </c>
       <c r="B75" s="3">
-        <v>7.08</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2281,7 +2293,7 @@
         <v>171</v>
       </c>
       <c r="B76" s="3">
-        <v>7.09</v>
+        <v>7.31</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2289,7 +2301,7 @@
         <v>172</v>
       </c>
       <c r="B77" s="3">
-        <v>6.94</v>
+        <v>7.06</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2297,7 +2309,7 @@
         <v>173</v>
       </c>
       <c r="B78" s="3">
-        <v>6.9</v>
+        <v>7.12</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2305,7 +2317,7 @@
         <v>174</v>
       </c>
       <c r="B79" s="3">
-        <v>6.8</v>
+        <v>6.88</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2313,7 +2325,7 @@
         <v>175</v>
       </c>
       <c r="B80" s="3">
-        <v>6.79</v>
+        <v>6.92</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2321,7 +2333,7 @@
         <v>176</v>
       </c>
       <c r="B81" s="3">
-        <v>6.66</v>
+        <v>6.71</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2329,7 +2341,7 @@
         <v>177</v>
       </c>
       <c r="B82" s="3">
-        <v>6.59</v>
+        <v>6.84</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2337,7 +2349,7 @@
         <v>178</v>
       </c>
       <c r="B83" s="3">
-        <v>6.53</v>
+        <v>6.55</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2345,7 +2357,7 @@
         <v>179</v>
       </c>
       <c r="B84" s="3">
-        <v>6.47</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2353,7 +2365,7 @@
         <v>180</v>
       </c>
       <c r="B85" s="3">
-        <v>6.33</v>
+        <v>6.48</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2361,7 +2373,7 @@
         <v>181</v>
       </c>
       <c r="B86" s="3">
-        <v>6.42</v>
+        <v>6.59</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2369,7 +2381,7 @@
         <v>182</v>
       </c>
       <c r="B87" s="3">
-        <v>6.3</v>
+        <v>6.33</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2377,7 +2389,7 @@
         <v>183</v>
       </c>
       <c r="B88" s="3">
-        <v>6.21</v>
+        <v>6.37</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2385,20 +2397,40 @@
         <v>184</v>
       </c>
       <c r="B89" s="3">
-        <v>6.17</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="2"/>
+      <c r="A90">
+        <v>185</v>
+      </c>
+      <c r="B90" s="2">
+        <v>6.21</v>
+      </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="2"/>
+      <c r="A91">
+        <v>186</v>
+      </c>
+      <c r="B91" s="2">
+        <v>5.96</v>
+      </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="2"/>
+      <c r="A92">
+        <v>187</v>
+      </c>
+      <c r="B92" s="2">
+        <v>6.12</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="2"/>
+      <c r="A93">
+        <v>188</v>
+      </c>
+      <c r="B93" s="2">
+        <v>5.83</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B94" s="2"/>

</xml_diff>